<commit_message>
primeiro teste com dash
</commit_message>
<xml_diff>
--- a/RELATORIOS.xlsx
+++ b/RELATORIOS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafael.cardoso\Documents\python\pandas_teste\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rfx\programacao\dash_python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91D2E3EE-B960-4FEA-BF58-16509A50FD4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6481D6D9-FA2F-49A5-ADAF-854FF836973D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="4" activeTab="9" xr2:uid="{B96B8094-1E43-4E68-ABC7-6E6983F80AC0}"/>
+    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{B96B8094-1E43-4E68-ABC7-6E6983F80AC0}"/>
   </bookViews>
   <sheets>
     <sheet name="FROTA VEICULOS" sheetId="1" r:id="rId1"/>
@@ -287,7 +287,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" indent="1"/>
@@ -362,9 +362,6 @@
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="3" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -751,30 +748,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="35"/>
-      <c r="E1" s="33">
+      <c r="C1" s="34"/>
+      <c r="E1" s="32">
         <v>44196</v>
       </c>
-      <c r="F1" s="34"/>
-      <c r="H1" s="33">
+      <c r="F1" s="33"/>
+      <c r="H1" s="32">
         <v>44561</v>
       </c>
-      <c r="I1" s="34"/>
-      <c r="K1" s="33">
+      <c r="I1" s="33"/>
+      <c r="K1" s="32">
         <v>44926</v>
       </c>
-      <c r="L1" s="34"/>
-      <c r="N1" s="33">
+      <c r="L1" s="33"/>
+      <c r="N1" s="32">
         <v>45291</v>
       </c>
-      <c r="O1" s="34"/>
-      <c r="Q1" s="33">
+      <c r="O1" s="33"/>
+      <c r="Q1" s="32">
         <v>45504</v>
       </c>
-      <c r="R1" s="34"/>
+      <c r="R1" s="33"/>
     </row>
     <row r="2" spans="2:18" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B2" s="8" t="s">
@@ -1482,7 +1479,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{700F9B68-8B51-4EC6-B8E6-93BA52DCC230}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1547,63 +1544,67 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFC0E34A-67F0-4F53-B77D-88A182D7921B}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
     <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="14">
+      <c r="B1" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="14">
         <v>2020</v>
       </c>
-      <c r="C1" s="14">
+      <c r="B2" s="28">
+        <v>23996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="14">
         <v>2021</v>
       </c>
-      <c r="D1" s="14">
+      <c r="B3" s="28">
+        <v>16018</v>
+      </c>
+      <c r="C3" s="27"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="14">
         <v>2022</v>
       </c>
-      <c r="E1" s="14">
+      <c r="B4" s="28">
+        <v>17252</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="14">
         <v>2023</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="B5" s="28">
+        <v>15751</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="29">
-        <v>23996</v>
-      </c>
-      <c r="C2" s="29">
-        <v>16018</v>
-      </c>
-      <c r="D2" s="29">
-        <v>17252</v>
-      </c>
-      <c r="E2" s="29">
-        <v>15751</v>
-      </c>
-      <c r="F2" s="29">
+      <c r="B6" s="28">
         <v>10764</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C3" s="27"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="28"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -1625,47 +1626,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="29" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="30">
+      <c r="A2" s="29">
         <v>2020</v>
       </c>
-      <c r="B2" s="31">
+      <c r="B2" s="30">
         <v>216088</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="30">
+      <c r="A3" s="29">
         <v>2021</v>
       </c>
-      <c r="B3" s="30">
+      <c r="B3" s="29">
         <v>215483</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="30">
+      <c r="A4" s="29">
         <v>2022</v>
       </c>
-      <c r="B4" s="30">
+      <c r="B4" s="29">
         <v>223654</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="30">
+      <c r="A5" s="29">
         <v>2023</v>
       </c>
-      <c r="B5" s="30">
+      <c r="B5" s="29">
         <v>243008</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="30">
+      <c r="A6" s="29">
         <v>2024</v>
       </c>
       <c r="B6">
@@ -1673,7 +1674,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="32"/>
+      <c r="A7" s="31"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -1684,8 +1685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE40917D-D5B0-46EE-A81B-D5B4B7FC3CA6}">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1695,10 +1696,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="33">
+      <c r="A1" s="32">
         <v>44196</v>
       </c>
-      <c r="B1" s="34"/>
+      <c r="B1" s="33"/>
     </row>
     <row r="2" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
@@ -1796,7 +1797,7 @@
         <v>2430</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>13</v>
       </c>
@@ -1804,7 +1805,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>14</v>
       </c>
@@ -1812,7 +1813,7 @@
         <v>30083</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>15</v>
       </c>
@@ -1820,7 +1821,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>16</v>
       </c>
@@ -1828,7 +1829,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>17</v>
       </c>
@@ -1868,10 +1869,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="33">
+      <c r="A1" s="32">
         <v>44561</v>
       </c>
-      <c r="B1" s="34"/>
+      <c r="B1" s="33"/>
     </row>
     <row r="2" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
@@ -2041,10 +2042,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="33">
+      <c r="A1" s="32">
         <v>44926</v>
       </c>
-      <c r="B1" s="34"/>
+      <c r="B1" s="33"/>
     </row>
     <row r="2" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
@@ -2214,10 +2215,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="33">
+      <c r="A1" s="32">
         <v>45291</v>
       </c>
-      <c r="B1" s="34"/>
+      <c r="B1" s="33"/>
     </row>
     <row r="2" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
@@ -2387,10 +2388,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="33">
+      <c r="A1" s="32">
         <v>45504</v>
       </c>
-      <c r="B1" s="34"/>
+      <c r="B1" s="33"/>
     </row>
     <row r="2" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
@@ -2549,7 +2550,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49868DFD-E911-4100-8E5B-21D6F166F464}">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
@@ -2560,10 +2561,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="35"/>
+      <c r="B1" s="34"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
@@ -2750,26 +2751,26 @@
     <row r="1" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
-      <c r="E1" s="33">
+      <c r="E1" s="32">
         <v>44196</v>
       </c>
-      <c r="F1" s="34"/>
-      <c r="H1" s="33">
+      <c r="F1" s="33"/>
+      <c r="H1" s="32">
         <v>44561</v>
       </c>
-      <c r="I1" s="34"/>
-      <c r="K1" s="33">
+      <c r="I1" s="33"/>
+      <c r="K1" s="32">
         <v>44926</v>
       </c>
-      <c r="L1" s="34"/>
-      <c r="N1" s="33">
+      <c r="L1" s="33"/>
+      <c r="N1" s="32">
         <v>45291</v>
       </c>
-      <c r="O1" s="34"/>
-      <c r="Q1" s="33">
+      <c r="O1" s="33"/>
+      <c r="Q1" s="32">
         <v>45504</v>
       </c>
-      <c r="R1" s="34"/>
+      <c r="R1" s="33"/>
     </row>
     <row r="2" spans="2:19" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
@@ -3555,8 +3556,8 @@
       </c>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B22" s="36"/>
-      <c r="C22" s="37"/>
+      <c r="B22" s="35"/>
+      <c r="C22" s="36"/>
     </row>
     <row r="23" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B23" s="16"/>

</xml_diff>

<commit_message>
finalizado do dia 03 de fevereiro de 2025
</commit_message>
<xml_diff>
--- a/RELATORIOS.xlsx
+++ b/RELATORIOS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rfx\programacao\dash_python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafael.cardoso\Documents\projetos\dash_python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9745E41A-464C-4472-9F25-B34FC9C9AFC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC465483-C13B-4A38-9549-5B211AEEF98C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="8" activeTab="11" xr2:uid="{B96B8094-1E43-4E68-ABC7-6E6983F80AC0}"/>
+    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="9" activeTab="11" xr2:uid="{B96B8094-1E43-4E68-ABC7-6E6983F80AC0}"/>
   </bookViews>
   <sheets>
     <sheet name="FROTA VEICULOS" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,8 @@
     <sheet name="CONDUTORES" sheetId="2" r:id="rId9"/>
     <sheet name="CONDUTORES POR ANO" sheetId="11" r:id="rId10"/>
     <sheet name="INFRAÇÕES" sheetId="3" r:id="rId11"/>
-    <sheet name="VEICULOS POR COMBUSTÍVEL" sheetId="12" r:id="rId12"/>
+    <sheet name="CONDUTORES POR CATEGORIA" sheetId="13" r:id="rId12"/>
+    <sheet name="VEICULOS POR COMBUSTÍVEL" sheetId="12" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,8 +39,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -47,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="58">
   <si>
     <t>Município</t>
   </si>
@@ -191,6 +190,36 @@
   </si>
   <si>
     <t>HIBRIDO</t>
+  </si>
+  <si>
+    <t>CATEGORIAS</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>AE</t>
+  </si>
+  <si>
+    <t>AD</t>
+  </si>
+  <si>
+    <t>AC</t>
+  </si>
+  <si>
+    <t>AB</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>A</t>
   </si>
 </sst>
 </file>
@@ -1599,7 +1628,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1664,10 +1693,109 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42713768-6072-452D-8523-9C96CA5F635E}">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2">
+        <v>3055</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4">
+        <v>77539</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6">
+        <v>13713</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7">
+        <v>12592</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8">
+        <v>2032</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9">
+        <v>68807</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10">
+        <v>6456</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBEE7320-D0F8-4761-B3D6-E94580B84941}">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>

</xml_diff>